<commit_message>
I am improving my technique
</commit_message>
<xml_diff>
--- a/CleanupExample.xlsx
+++ b/CleanupExample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F931A7E9-7303-4D43-8BDC-7378CD45515B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{628AF060-B14A-43E9-B751-404B6B75E217}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
@@ -1612,7 +1612,7 @@
   </sheetPr>
   <dimension ref="A1:BA136"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="C19" sqref="C19:F25"/>
     </sheetView>
   </sheetViews>
@@ -2982,8 +2982,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37937A3D-90F8-4290-B85F-D4D4A3914864}">
   <dimension ref="A3:BF96"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>

</xml_diff>